<commit_message>
Modified versions of courses.py and pupils.py. Also many fiels in transition ...
</commit_message>
<xml_diff>
--- a/TESTDATA/RESOURCES/templates/Noten/Noteneingabe-Abitur.xlsx
+++ b/TESTDATA/RESOURCES/templates/Noten/Noteneingabe-Abitur.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Schüler(in)</t>
   </si>
   <si>
-    <t xml:space="preserve">Maßstab</t>
+    <t xml:space="preserve">Gruppen</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
@@ -401,10 +401,10 @@
   <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.74"/>
@@ -2189,14 +2189,14 @@
     <mergeCell ref="J4:O4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11:AD52" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11:AD52" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,*,/"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.636805555555555" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>